<commit_message>
[Sanity] Configure sanityCMS into project
Include switch between excel and sanity data source
</commit_message>
<xml_diff>
--- a/public/jargon_and_acronyms.xlsx
+++ b/public/jargon_and_acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brendan.campbell/source/personal/jargon-buster/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF01FFC2-93FC-B641-BDC5-956801CBA8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496D25ED-8392-DD4E-8081-21F3C98500F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{E5626C7C-A339-EF44-9421-6BA264895E86}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="315">
   <si>
     <t>Term</t>
   </si>
@@ -1412,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B8514E-7BB7-5448-92A7-AC2D3CACAF56}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1549,9 +1549,6 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
       <c r="B9" t="s">
         <v>271</v>
       </c>

</xml_diff>